<commit_message>
Clean Create Pkg and parameratized
</commit_message>
<xml_diff>
--- a/Eclipse2022-03/Eclipse2022-03_Jul2522/Default.xlsx
+++ b/Eclipse2022-03/Eclipse2022-03_Jul2522/Default.xlsx
@@ -19,9 +19,45 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="13">
+  <si>
+    <t>p_ZMF_Applications</t>
+  </si>
+  <si>
+    <t>ChangeMan ZMF4ECL Version(8.3.0.625202207131302);A004-ZMFQSH - ZMF Version(8.2.0.6)</t>
+  </si>
+  <si>
+    <t>p_ZMF_A004-SH_Connected</t>
+  </si>
+  <si>
+    <t>ChangeMan ZMF4ECL Version(8.3.0.625202207131302);A004-ZMFQSH - ZMF Version(8.2.0.6);ZMF Applications;Default Application Folder;SAN1 - Sanity Testing Application</t>
+  </si>
+  <si>
+    <t>ChangeMan ZMF4ECL Version(8.3.0.625202207131302);A004-ZMFQSH</t>
+  </si>
+  <si>
+    <t>ChangeMan ZMF4ECL Version(8.3.0.625202207131302);A004-ZMFQSH - ZMF Version(8.2.0.6);ZMF Applications</t>
+  </si>
+  <si>
+    <t>ChangeMan ZMF4ECL Version(8.3.0.625202207131302);A004-ZMFQSH - ZMF Version(8.2.0.6);ZMF Applications;Default Application Folder</t>
+  </si>
+  <si>
+    <t>CMN2100I_PkgName</t>
+  </si>
   <si>
     <t>NewPkgName</t>
+  </si>
+  <si>
+    <t>p_ZMF_A004-SH</t>
+  </si>
+  <si>
+    <t>p_ZMF_App_DefaultFolder</t>
+  </si>
+  <si>
+    <t>p_ZMF_A004-SH_SAN1</t>
+  </si>
+  <si>
+    <t>CMN2100I - SAN1000128 change package has been created.</t>
   </si>
 </sst>
 </file>
@@ -166,7 +202,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -174,13 +210,43 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -479,21 +545,68 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A1" sqref="A1:G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.1"/>
   <cols>
-    <col min="1" max="1" width="12.91796875" style="1" customWidth="1"/>
-    <col min="2" max="16384" width="9.078125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="53.0078125" style="2" customWidth="1"/>
+    <col min="2" max="3" width="20.31640625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="16.27734375" style="2" customWidth="1"/>
+    <col min="5" max="5" width="9.41796875" style="2" customWidth="1"/>
+    <col min="6" max="6" width="21.1171875" style="2" customWidth="1"/>
+    <col min="7" max="7" width="9.41796875" style="2" customWidth="1"/>
+    <col min="8" max="16384" width="9.078125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="14.95" customFormat="1">
+    <row r="1" customFormat="1">
       <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" t="s">
         <v>0</v>
+      </c>
+      <c r="E1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="1" t="str">
+        <f>TRIM(MID(SUBSTITUTE(A2," ",REPT(" ",LEN(A2))), (3-1)*LEN(A2)+1, LEN(A2)))</f>
+        <v>SAN1000128</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -511,8 +624,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.1"/>
   <cols>
-    <col min="1" max="1" width="9.41796875" style="1" customWidth="1"/>
-    <col min="2" max="16384" width="9.078125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="9.41796875" style="2" customWidth="1"/>
+    <col min="2" max="16384" width="9.078125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.95" customFormat="1"/>
@@ -531,7 +644,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.1"/>
   <cols>
-    <col min="1" max="16384" width="9.078125" style="1" customWidth="1"/>
+    <col min="1" max="16384" width="9.078125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.95" customFormat="1"/>
@@ -550,7 +663,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.1"/>
   <cols>
-    <col min="1" max="16384" width="9.078125" style="1" customWidth="1"/>
+    <col min="1" max="16384" width="9.078125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.95" customFormat="1"/>
@@ -569,7 +682,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.1"/>
   <cols>
-    <col min="1" max="16384" width="9.078125" style="1" customWidth="1"/>
+    <col min="1" max="16384" width="9.078125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.95" customFormat="1"/>
@@ -588,7 +701,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.1"/>
   <cols>
-    <col min="1" max="16384" width="9.078125" style="1" customWidth="1"/>
+    <col min="1" max="16384" width="9.078125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.95" customFormat="1"/>

</xml_diff>